<commit_message>
Minor Update + Merge from Khang
</commit_message>
<xml_diff>
--- a/AutomatedData_#1.xlsx
+++ b/AutomatedData_#1.xlsx
@@ -74,7 +74,7 @@
     <t>GPU Decoding</t>
   </si>
   <si>
-    <t>cuda</t>
+    <t>Cuda</t>
   </si>
   <si>
     <t>H264</t>
@@ -115,7 +115,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -125,11 +125,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD3D3D3" tint="0"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF778899" tint="0"/>
       </patternFill>
     </fill>
     <fill>
@@ -165,7 +160,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -174,7 +169,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -185,6 +179,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr codeName=""/>
   <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -272,13 +267,13 @@
       <c r="D2" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="3" t="s">
+      <c r="E2" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>21</v>
       </c>
       <c r="H2" s="0" t="s">
@@ -287,8 +282,11 @@
       <c r="I2" s="0" t="s">
         <v>23</v>
       </c>
+      <c r="J2" s="0">
+        <v>225</v>
+      </c>
       <c r="K2" s="0">
-        <v>17.885217666625977</v>
+        <v>76.48353576660156</v>
       </c>
       <c r="L2" s="0">
         <v>0</v>
@@ -319,13 +317,13 @@
       <c r="D3" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" s="3" t="s">
+      <c r="E3" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>21</v>
       </c>
       <c r="H3" s="0" t="s">
@@ -334,8 +332,11 @@
       <c r="I3" s="0" t="s">
         <v>24</v>
       </c>
+      <c r="J3" s="0">
+        <v>742</v>
+      </c>
       <c r="K3" s="0">
-        <v>8.103363990783691</v>
+        <v>89.66920471191406</v>
       </c>
       <c r="L3" s="0">
         <v>0</v>
@@ -366,13 +367,13 @@
       <c r="D4" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="3" t="s">
+      <c r="E4" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="3" t="s">
         <v>21</v>
       </c>
       <c r="H4" s="0" t="s">
@@ -381,8 +382,11 @@
       <c r="I4" s="0" t="s">
         <v>23</v>
       </c>
+      <c r="J4" s="0">
+        <v>223</v>
+      </c>
       <c r="K4" s="0">
-        <v>8.063426971435547</v>
+        <v>96.89981842041016</v>
       </c>
       <c r="L4" s="0">
         <v>0</v>
@@ -413,13 +417,13 @@
       <c r="D5" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="3" t="s">
+      <c r="E5" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="3" t="s">
         <v>21</v>
       </c>
       <c r="H5" s="0" t="s">
@@ -428,8 +432,11 @@
       <c r="I5" s="0" t="s">
         <v>24</v>
       </c>
+      <c r="J5" s="0">
+        <v>738</v>
+      </c>
       <c r="K5" s="0">
-        <v>7.13214635848999</v>
+        <v>96.77064514160156</v>
       </c>
       <c r="L5" s="0">
         <v>0</v>
@@ -460,13 +467,13 @@
       <c r="D6" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="5" t="s">
+      <c r="E6" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="3" t="s">
         <v>21</v>
       </c>
       <c r="H6" s="0" t="s">
@@ -475,8 +482,11 @@
       <c r="I6" s="0" t="s">
         <v>23</v>
       </c>
+      <c r="J6" s="0">
+        <v>120</v>
+      </c>
       <c r="K6" s="0">
-        <v>5.585605144500732</v>
+        <v>47.747337341308594</v>
       </c>
       <c r="L6" s="0">
         <v>0</v>
@@ -507,13 +517,13 @@
       <c r="D7" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="5" t="s">
+      <c r="E7" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="3" t="s">
         <v>21</v>
       </c>
       <c r="H7" s="0" t="s">
@@ -522,8 +532,11 @@
       <c r="I7" s="0" t="s">
         <v>24</v>
       </c>
+      <c r="J7" s="0">
+        <v>237</v>
+      </c>
       <c r="K7" s="0">
-        <v>5.553906440734863</v>
+        <v>24.257783889770508</v>
       </c>
       <c r="L7" s="0">
         <v>0</v>
@@ -554,13 +567,13 @@
       <c r="D8" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" s="5" t="s">
+      <c r="E8" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="3" t="s">
         <v>21</v>
       </c>
       <c r="H8" s="0" t="s">
@@ -569,14 +582,17 @@
       <c r="I8" s="0" t="s">
         <v>23</v>
       </c>
+      <c r="J8" s="0">
+        <v>119</v>
+      </c>
       <c r="K8" s="0">
-        <v>7.709231853485107</v>
+        <v>48.50333786010742</v>
       </c>
       <c r="L8" s="0">
-        <v>0.9494950771331787</v>
+        <v>0</v>
       </c>
       <c r="M8" s="0">
-        <v>0.9494950771331787</v>
+        <v>0</v>
       </c>
       <c r="N8" s="0">
         <v>0</v>
@@ -601,13 +617,13 @@
       <c r="D9" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" s="5" t="s">
+      <c r="E9" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" s="3" t="s">
         <v>21</v>
       </c>
       <c r="H9" s="0" t="s">
@@ -616,8 +632,11 @@
       <c r="I9" s="0" t="s">
         <v>24</v>
       </c>
+      <c r="J9" s="0">
+        <v>237</v>
+      </c>
       <c r="K9" s="0">
-        <v>4.482483386993408</v>
+        <v>27.65400505065918</v>
       </c>
       <c r="L9" s="0">
         <v>0</v>
@@ -648,13 +667,13 @@
       <c r="D10" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F10" s="5" t="s">
+      <c r="E10" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="G10" s="5" t="s">
         <v>27</v>
       </c>
       <c r="H10" s="0" t="s">
@@ -663,8 +682,11 @@
       <c r="I10" s="0" t="s">
         <v>23</v>
       </c>
+      <c r="J10" s="0">
+        <v>91</v>
+      </c>
       <c r="K10" s="0">
-        <v>7.889227390289307</v>
+        <v>48.77279281616211</v>
       </c>
       <c r="L10" s="0">
         <v>0</v>
@@ -695,13 +717,13 @@
       <c r="D11" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F11" s="5" t="s">
+      <c r="E11" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G11" s="5" t="s">
         <v>27</v>
       </c>
       <c r="H11" s="0" t="s">
@@ -710,14 +732,17 @@
       <c r="I11" s="0" t="s">
         <v>24</v>
       </c>
+      <c r="J11" s="0">
+        <v>198</v>
+      </c>
       <c r="K11" s="0">
-        <v>5.793210506439209</v>
+        <v>26.671972274780273</v>
       </c>
       <c r="L11" s="0">
-        <v>0.9906152486801147</v>
+        <v>0</v>
       </c>
       <c r="M11" s="0">
-        <v>0.9906152486801147</v>
+        <v>0</v>
       </c>
       <c r="N11" s="0">
         <v>0</v>
@@ -742,13 +767,13 @@
       <c r="D12" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F12" s="5" t="s">
+      <c r="E12" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="G12" s="5" t="s">
         <v>27</v>
       </c>
       <c r="H12" s="0" t="s">
@@ -757,14 +782,17 @@
       <c r="I12" s="0" t="s">
         <v>23</v>
       </c>
+      <c r="J12" s="0">
+        <v>91</v>
+      </c>
       <c r="K12" s="0">
-        <v>4.683475971221924</v>
+        <v>46.7420654296875</v>
       </c>
       <c r="L12" s="0">
-        <v>2.8408241271972656</v>
+        <v>0</v>
       </c>
       <c r="M12" s="0">
-        <v>2.8408241271972656</v>
+        <v>0</v>
       </c>
       <c r="N12" s="0">
         <v>0</v>
@@ -789,13 +817,13 @@
       <c r="D13" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="E13" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F13" s="5" t="s">
+      <c r="E13" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="5" t="s">
         <v>27</v>
       </c>
       <c r="H13" s="0" t="s">
@@ -804,14 +832,17 @@
       <c r="I13" s="0" t="s">
         <v>24</v>
       </c>
+      <c r="J13" s="0">
+        <v>198</v>
+      </c>
       <c r="K13" s="0">
-        <v>6.6582794189453125</v>
+        <v>27.22649383544922</v>
       </c>
       <c r="L13" s="0">
-        <v>0.6640614867210388</v>
+        <v>0</v>
       </c>
       <c r="M13" s="0">
-        <v>0.6640614867210388</v>
+        <v>0</v>
       </c>
       <c r="N13" s="0">
         <v>0</v>
@@ -836,7 +867,7 @@
       <c r="D14" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="0" t="s">
         <v>19</v>
       </c>
       <c r="F14" s="0" t="s">
@@ -851,8 +882,11 @@
       <c r="I14" s="0" t="s">
         <v>28</v>
       </c>
+      <c r="J14" s="0">
+        <v>-1</v>
+      </c>
       <c r="K14" s="0">
-        <v>6.54910135269165</v>
+        <v>2.983180522918701</v>
       </c>
       <c r="L14" s="0">
         <v>0</v>
@@ -883,7 +917,7 @@
       <c r="D15" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E15" s="0" t="s">
         <v>19</v>
       </c>
       <c r="F15" s="0" t="s">
@@ -898,8 +932,11 @@
       <c r="I15" s="0" t="s">
         <v>28</v>
       </c>
+      <c r="J15" s="0">
+        <v>-1</v>
+      </c>
       <c r="K15" s="0">
-        <v>6.107327938079834</v>
+        <v>0.9193068742752075</v>
       </c>
       <c r="L15" s="0">
         <v>0</v>

</xml_diff>